<commit_message>
Worked on lesson page
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anita\OneDrive\Documents\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0307983E-54B1-4AB4-80E1-730B951ACB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB16326-DBC1-43F4-B61F-D1DD8A3FA996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{282B6C35-1778-45D6-BBF2-0E4A250752AB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>TC_ID</t>
   </si>
@@ -60,122 +60,206 @@
     <t>Remark/Suggestion</t>
   </si>
   <si>
-    <t>TC_001</t>
-  </si>
-  <si>
-    <t>Req_001</t>
-  </si>
-  <si>
     <t>Functionality</t>
   </si>
   <si>
     <t>Must be</t>
   </si>
   <si>
-    <t>Admin Login</t>
-  </si>
-  <si>
-    <t>Admin should be able to log in to the admin dashboard.</t>
-  </si>
-  <si>
-    <t>Admin login page should not be visible to users; admin must have valid credentials.</t>
-  </si>
-  <si>
-    <t>Successfully logged in and redirected to the dashboard.</t>
-  </si>
-  <si>
     <t>Fulfilled</t>
   </si>
   <si>
-    <t>TC_002</t>
-  </si>
-  <si>
-    <t>Req_002</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>Req_003</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>Req_004</t>
-  </si>
-  <si>
-    <t>User Sign-Up</t>
-  </si>
-  <si>
     <t>Users should be able to register for an account.</t>
   </si>
   <si>
-    <t>The signup page should be accessible, and users must provide valid information.</t>
-  </si>
-  <si>
-    <t>Successfully registered the user account.</t>
-  </si>
-  <si>
-    <t>User Login</t>
-  </si>
-  <si>
-    <t>Users should be able to log in to their accounts.</t>
-  </si>
-  <si>
-    <t>Users should have a valid account and be on the login page.</t>
-  </si>
-  <si>
-    <t>Successfully logged in and redirected to the homepage.</t>
-  </si>
-  <si>
-    <t>User Logout</t>
-  </si>
-  <si>
-    <t>Users should be able to log out after logging in.</t>
-  </si>
-  <si>
-    <t>Users must be logged in to access the logout option.</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Successfully logged out and redirected to the login page.</t>
   </si>
   <si>
-    <t>1. Navigate to /admin in the URL. 2. Enter admin username and password. 3. Click on Log In.</t>
-  </si>
-  <si>
-    <t>1. Navigate to the signup page. 2. Fill in required fields (username, email, password). 3. Click Sign Up.</t>
-  </si>
-  <si>
-    <t>1. Navigate to the login page. 2. Enter valid username and password. 3. Click Log In.</t>
-  </si>
-  <si>
-    <t>1. Click on the Logout button in the user profile. 2. Confirm the logout prompt if available.</t>
-  </si>
-  <si>
-    <t>Username: admin</t>
-  </si>
-  <si>
-    <t>Password: anita1234</t>
-  </si>
-  <si>
-    <t>Email: ram1234@gmail.com</t>
-  </si>
-  <si>
-    <t>Username: ram</t>
-  </si>
-  <si>
-    <t>Password: ram12345</t>
+    <t>TC_UM_001</t>
+  </si>
+  <si>
+    <t>UMS_F_001</t>
+  </si>
+  <si>
+    <t>User Self-Registration</t>
+  </si>
+  <si>
+    <t>Signup page should be accessible, and user must enter valid info.</t>
+  </si>
+  <si>
+    <t>1. Navigate to the signup page.
+2. Fill in username, email, password.
+3. Click "Sign Up".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: Pixie
+Email: pixiewalker000@gmail.com
+</t>
+  </si>
+  <si>
+    <t>User account is created successfully.</t>
+  </si>
+  <si>
+    <t>TC_UM_002</t>
+  </si>
+  <si>
+    <t>User must verify email to proceed to login.</t>
+  </si>
+  <si>
+    <t>Email Verification with OTP</t>
+  </si>
+  <si>
+    <t>1. After sign up, prompt for OTP.
+2. OTP is sent via email.
+3. Enter OTP and submit.</t>
+  </si>
+  <si>
+    <t>User must have completed registration.</t>
+  </si>
+  <si>
+    <t>In-progress</t>
+  </si>
+  <si>
+    <t>TC_UM_003</t>
+  </si>
+  <si>
+    <t>TC_UM_004</t>
+  </si>
+  <si>
+    <t>TC_UM_005</t>
+  </si>
+  <si>
+    <t>TC_UM_006</t>
+  </si>
+  <si>
+    <t>TC_UM_007</t>
+  </si>
+  <si>
+    <t>UMS_F_002</t>
+  </si>
+  <si>
+    <t>UMS_F_003</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>UMS_NF_004</t>
+  </si>
+  <si>
+    <t>UMS_NF_005</t>
+  </si>
+  <si>
+    <t>UMS_NF_006</t>
+  </si>
+  <si>
+    <t>UMS_NF_007</t>
+  </si>
+  <si>
+    <t>Should be</t>
+  </si>
+  <si>
+    <t>View Profile After Login</t>
+  </si>
+  <si>
+    <t>Password Encryption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Dashboard Access Post Login</t>
+  </si>
+  <si>
+    <t>Edit Profile</t>
+  </si>
+  <si>
+    <t>Admin Access to Content Panel</t>
+  </si>
+  <si>
+    <t>Users should be able to view their profile.</t>
+  </si>
+  <si>
+    <t>Passwords should be stored securely.</t>
+  </si>
+  <si>
+    <t>Users should access lessons post-login.</t>
+  </si>
+  <si>
+    <t>Users should be able to update profile info.</t>
+  </si>
+  <si>
+    <t>Admin should be able to access content management.</t>
+  </si>
+  <si>
+    <t>User must be logged in.</t>
+  </si>
+  <si>
+    <t>Signup form submitted.</t>
+  </si>
+  <si>
+    <t>User should be logged in.</t>
+  </si>
+  <si>
+    <t>Logged in as Admin</t>
+  </si>
+  <si>
+    <t>1. Login to account.
+2. Navigate to profile page.</t>
+  </si>
+  <si>
+    <t>1. Submit signup form.
+2. Check database storage format.</t>
+  </si>
+  <si>
+    <t>1. Login successfully.
+2. Navigate to dashboard.
+3. Check lesson visibility.</t>
+  </si>
+  <si>
+    <t>1. Go to profile.
+2. Edit name/email.
+3. Save changes.</t>
+  </si>
+  <si>
+    <t>1. Login as admin.
+2. Navigate to /admin/content.</t>
+  </si>
+  <si>
+    <t>Password: pixie@123</t>
+  </si>
+  <si>
+    <t>Password:  pixie@123</t>
+  </si>
+  <si>
+    <t>Username: Pixie
+Password: pixie@123</t>
+  </si>
+  <si>
+    <t>New name: PiXie</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin@123</t>
+  </si>
+  <si>
+    <t>Profile data (name, email, progress) is visible.</t>
+  </si>
+  <si>
+    <t>Password stored in bcrypt-hashed format.</t>
+  </si>
+  <si>
+    <t>Dashboard and lessons loaded successfully.</t>
+  </si>
+  <si>
+    <t>Profile updated successfully.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +279,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -304,6 +394,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -313,10 +407,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -633,284 +723,366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CC1566-696A-4EA6-95FE-A374B1BFA9A7}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="25.77734375" customWidth="1"/>
     <col min="10" max="10" width="17.5546875" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6"/>
+      <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="129.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:12" ht="75.599999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>19</v>
+      <c r="J4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
@@ -921,7 +1093,28 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>